<commit_message>
[labb1] Fixat diagram i rapporten.
</commit_message>
<xml_diff>
--- a/Execution.xlsx
+++ b/Execution.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20225"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="1620" yWindow="0" windowWidth="25600" windowHeight="19020" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="1620" yWindow="0" windowWidth="19440" windowHeight="12240" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -12,6 +12,7 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$C$14</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Sheet2!$A$1:$C$1</definedName>
   </definedNames>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
@@ -23,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="7">
   <si>
     <t>Cores</t>
   </si>
@@ -31,52 +32,10 @@
     <t>Execution time</t>
   </si>
   <si>
-    <t>0.51679</t>
-  </si>
-  <si>
-    <t>0.78802</t>
-  </si>
-  <si>
     <t>Radius</t>
   </si>
   <si>
-    <t>0.357867</t>
-  </si>
-  <si>
-    <t>0.140421</t>
-  </si>
-  <si>
-    <t>0.0883818</t>
-  </si>
-  <si>
-    <t>0.77188</t>
-  </si>
-  <si>
-    <t>1.04383</t>
-  </si>
-  <si>
-    <t>0.0334301</t>
-  </si>
-  <si>
-    <t>0.0198572</t>
-  </si>
-  <si>
-    <t>0.0251968</t>
-  </si>
-  <si>
-    <t>0.0851059</t>
-  </si>
-  <si>
-    <t>0.278635</t>
-  </si>
-  <si>
-    <t>0.647985</t>
-  </si>
-  <si>
     <t>Bild</t>
-  </si>
-  <si>
-    <t>0.034184</t>
   </si>
   <si>
     <t>im1</t>
@@ -85,58 +44,7 @@
     <t>im2</t>
   </si>
   <si>
-    <t>0.0137081</t>
-  </si>
-  <si>
     <t>im3</t>
-  </si>
-  <si>
-    <t>0.0128999</t>
-  </si>
-  <si>
-    <t>0.028933</t>
-  </si>
-  <si>
-    <t>0.0131681</t>
-  </si>
-  <si>
-    <t>0.0129931</t>
-  </si>
-  <si>
-    <t>0.0379179</t>
-  </si>
-  <si>
-    <t>0.0148308</t>
-  </si>
-  <si>
-    <t>0.0138838</t>
-  </si>
-  <si>
-    <t>0.076829</t>
-  </si>
-  <si>
-    <t>0.0541761</t>
-  </si>
-  <si>
-    <t>0.050391</t>
-  </si>
-  <si>
-    <t>0.117357</t>
-  </si>
-  <si>
-    <t>0.0985909</t>
-  </si>
-  <si>
-    <t>0.0873239</t>
-  </si>
-  <si>
-    <t>0.325144</t>
-  </si>
-  <si>
-    <t>0.219953</t>
-  </si>
-  <si>
-    <t>0.293217</t>
   </si>
 </sst>
 </file>
@@ -223,39 +131,621 @@
     </xf>
   </cellXfs>
   <cellStyles count="29">
-    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="16" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="18" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="20" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="22" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="24" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="26" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="28" builtinId="9" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="13" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="15" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="17" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="19" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="21" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="23" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="25" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="27" builtinId="8" hidden="1"/>
+    <cellStyle name="Följd hyperlänk" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Följd hyperlänk" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Följd hyperlänk" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Följd hyperlänk" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="Följd hyperlänk" xfId="10" builtinId="9" hidden="1"/>
+    <cellStyle name="Följd hyperlänk" xfId="12" builtinId="9" hidden="1"/>
+    <cellStyle name="Följd hyperlänk" xfId="14" builtinId="9" hidden="1"/>
+    <cellStyle name="Följd hyperlänk" xfId="16" builtinId="9" hidden="1"/>
+    <cellStyle name="Följd hyperlänk" xfId="18" builtinId="9" hidden="1"/>
+    <cellStyle name="Följd hyperlänk" xfId="20" builtinId="9" hidden="1"/>
+    <cellStyle name="Följd hyperlänk" xfId="22" builtinId="9" hidden="1"/>
+    <cellStyle name="Följd hyperlänk" xfId="24" builtinId="9" hidden="1"/>
+    <cellStyle name="Följd hyperlänk" xfId="26" builtinId="9" hidden="1"/>
+    <cellStyle name="Följd hyperlänk" xfId="28" builtinId="9" hidden="1"/>
+    <cellStyle name="Hyperlänk" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlänk" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlänk" xfId="5" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlänk" xfId="7" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlänk" xfId="9" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlänk" xfId="11" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlänk" xfId="13" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlänk" xfId="15" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlänk" xfId="17" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlänk" xfId="19" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlänk" xfId="21" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlänk" xfId="23" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlänk" xfId="25" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlänk" xfId="27" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="sv-SE"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>8 Kärnor</c:v>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet1!$C$2:$C$5</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>50</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$B$2:$B$5</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>3.3430099999999997E-2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.14042099999999999</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.51678999999999997</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.04383</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>16 Kärnor</c:v>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet1!$C$2:$C$5</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>50</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$B$6:$B$9</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>1.9857199999999998E-2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>8.8381799999999996E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.35786699999999999</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.78802000000000005</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:v>32 Kärnor</c:v>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet1!$C$2:$C$5</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>50</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$B$11:$B$14</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>2.5196799999999998E-2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>8.5105899999999998E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.27863500000000002</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.64798500000000003</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="150"/>
+        <c:axId val="90840064"/>
+        <c:axId val="70574848"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="90840064"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="70574848"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="70574848"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="90840064"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="sv-SE"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>Bild 1</c:v>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet2!$A$8:$A$13</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>160</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>240</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>400</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet2!$B$2:$B$7</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>3.4183999999999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2.8933E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3.7917899999999997E-2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>7.6828999999999995E-2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.117357</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.32514399999999999</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>Bild 2</c:v>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet2!$A$8:$A$13</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>160</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>240</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>400</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet2!$B$8:$B$13</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>1.3708100000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.31681E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.48308E-2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>5.4176099999999998E-2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>9.8590899999999995E-2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.21995300000000001</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:v>Bild 3</c:v>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet2!$A$8:$A$13</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>160</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>240</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>400</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet2!$B$14:$B$19</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>1.2899900000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.29931E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.38838E-2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>5.0390999999999998E-2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>8.7323899999999996E-2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.29321700000000001</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="150"/>
+        <c:axId val="32750592"/>
+        <c:axId val="32752384"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="32750592"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="32752384"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="32752384"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="0.30000000000000004"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="General" sourceLinked="0"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="32750592"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>790575</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>157162</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>333375</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>100012</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Diagram 1" title="Exekveringstid blurfilter"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>676275</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>47625</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>219075</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>190500</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="4" name="Diagram 3"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -582,16 +1072,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A17" sqref="A17"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="16.33203125" customWidth="1"/>
+    <col min="2" max="2" width="16.375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -599,159 +1089,155 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>8</v>
       </c>
-      <c r="B2" s="1" t="s">
-        <v>10</v>
+      <c r="B2" s="1">
+        <v>3.3430099999999997E-2</v>
       </c>
       <c r="C2">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>8</v>
       </c>
-      <c r="B3" s="1" t="s">
-        <v>6</v>
+      <c r="B3" s="1">
+        <v>0.14042099999999999</v>
       </c>
       <c r="C3">
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>8</v>
       </c>
-      <c r="B4" s="1" t="s">
-        <v>2</v>
+      <c r="B4" s="1">
+        <v>0.51678999999999997</v>
       </c>
       <c r="C4">
         <v>30</v>
       </c>
     </row>
-    <row r="5" spans="1:3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>8</v>
       </c>
-      <c r="B5" s="1" t="s">
-        <v>9</v>
+      <c r="B5" s="1">
+        <v>1.04383</v>
       </c>
       <c r="C5">
         <v>50</v>
       </c>
     </row>
-    <row r="6" spans="1:3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>16</v>
       </c>
-      <c r="B6" s="1" t="s">
-        <v>11</v>
+      <c r="B6" s="1">
+        <v>1.9857199999999998E-2</v>
       </c>
       <c r="C6">
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>16</v>
       </c>
-      <c r="B7" s="1" t="s">
-        <v>7</v>
+      <c r="B7" s="1">
+        <v>8.8381799999999996E-2</v>
       </c>
       <c r="C7">
         <v>10</v>
       </c>
     </row>
-    <row r="8" spans="1:3">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>16</v>
       </c>
-      <c r="B8" s="1" t="s">
-        <v>5</v>
+      <c r="B8" s="1">
+        <v>0.35786699999999999</v>
       </c>
       <c r="C8">
         <v>30</v>
       </c>
     </row>
-    <row r="9" spans="1:3">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>16</v>
       </c>
-      <c r="B9" s="1" t="s">
-        <v>3</v>
+      <c r="B9" s="1">
+        <v>0.78802000000000005</v>
       </c>
       <c r="C9">
         <v>50</v>
       </c>
     </row>
-    <row r="10" spans="1:3">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>16</v>
       </c>
-      <c r="B10" s="1" t="s">
-        <v>8</v>
+      <c r="B10" s="1">
+        <v>0.77188000000000001</v>
       </c>
       <c r="C10">
         <v>50</v>
       </c>
     </row>
-    <row r="11" spans="1:3">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>32</v>
       </c>
-      <c r="B11" s="1" t="s">
-        <v>12</v>
+      <c r="B11" s="1">
+        <v>2.5196799999999998E-2</v>
       </c>
       <c r="C11">
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:3">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>32</v>
       </c>
-      <c r="B12" s="1" t="s">
-        <v>13</v>
+      <c r="B12" s="1">
+        <v>8.5105899999999998E-2</v>
       </c>
       <c r="C12">
         <v>10</v>
       </c>
     </row>
-    <row r="13" spans="1:3">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>32</v>
       </c>
-      <c r="B13" s="1" t="s">
-        <v>14</v>
+      <c r="B13" s="1">
+        <v>0.27863500000000002</v>
       </c>
       <c r="C13">
         <v>30</v>
       </c>
     </row>
-    <row r="14" spans="1:3">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>32</v>
       </c>
-      <c r="B14" s="1" t="s">
-        <v>15</v>
+      <c r="B14" s="1">
+        <v>0.64798500000000003</v>
       </c>
       <c r="C14">
         <v>50</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:C14">
-    <sortState ref="A2:C14">
-      <sortCondition ref="A1:A14"/>
-    </sortState>
-  </autoFilter>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <drawing r:id="rId1"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
@@ -764,16 +1250,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E18" sqref="E18"/>
+    <sheetView topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="K16" sqref="K16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="17.83203125" customWidth="1"/>
+    <col min="2" max="2" width="17.875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -781,209 +1267,213 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>8</v>
       </c>
-      <c r="B2" t="s">
-        <v>17</v>
+      <c r="B2">
+        <v>3.4183999999999999E-2</v>
       </c>
       <c r="C2" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3">
+        <v>16</v>
+      </c>
+      <c r="B3">
+        <v>2.8933E-2</v>
+      </c>
+      <c r="C3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>32</v>
+      </c>
+      <c r="B4">
+        <v>3.7917899999999997E-2</v>
+      </c>
+      <c r="C4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>160</v>
+      </c>
+      <c r="B5">
+        <v>7.6828999999999995E-2</v>
+      </c>
+      <c r="C5" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>240</v>
+      </c>
+      <c r="B6">
+        <v>0.117357</v>
+      </c>
+      <c r="C6" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>400</v>
+      </c>
+      <c r="B7">
+        <v>0.32514399999999999</v>
+      </c>
+      <c r="C7" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8">
         <v>8</v>
       </c>
-      <c r="B3" t="s">
-        <v>20</v>
-      </c>
-      <c r="C3" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3">
-      <c r="A4">
-        <v>8</v>
-      </c>
-      <c r="B4" t="s">
-        <v>22</v>
-      </c>
-      <c r="C4" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3">
-      <c r="A5">
+      <c r="B8">
+        <v>1.3708100000000001E-2</v>
+      </c>
+      <c r="C8" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9">
         <v>16</v>
       </c>
-      <c r="B5" t="s">
-        <v>23</v>
-      </c>
-      <c r="C5" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3">
-      <c r="A6">
-        <v>16</v>
-      </c>
-      <c r="B6" t="s">
-        <v>24</v>
-      </c>
-      <c r="C6" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3">
-      <c r="A7">
-        <v>16</v>
-      </c>
-      <c r="B7" t="s">
-        <v>25</v>
-      </c>
-      <c r="C7" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3">
-      <c r="A8">
-        <v>32</v>
-      </c>
-      <c r="B8" t="s">
-        <v>26</v>
-      </c>
-      <c r="C8" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3">
-      <c r="A9">
-        <v>32</v>
-      </c>
-      <c r="B9" t="s">
-        <v>27</v>
+      <c r="B9">
+        <v>1.31681E-2</v>
       </c>
       <c r="C9" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>32</v>
       </c>
-      <c r="B10" t="s">
-        <v>28</v>
+      <c r="B10">
+        <v>1.48308E-2</v>
       </c>
       <c r="C10" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>160</v>
       </c>
-      <c r="B11" t="s">
-        <v>29</v>
+      <c r="B11">
+        <v>5.4176099999999998E-2</v>
       </c>
       <c r="C11" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12">
+        <v>240</v>
+      </c>
+      <c r="B12">
+        <v>9.8590899999999995E-2</v>
+      </c>
+      <c r="C12" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>400</v>
+      </c>
+      <c r="B13">
+        <v>0.21995300000000001</v>
+      </c>
+      <c r="C13" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>8</v>
+      </c>
+      <c r="B14">
+        <v>1.2899900000000001E-2</v>
+      </c>
+      <c r="C14" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>16</v>
+      </c>
+      <c r="B15">
+        <v>1.29931E-2</v>
+      </c>
+      <c r="C15" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>32</v>
+      </c>
+      <c r="B16">
+        <v>1.38838E-2</v>
+      </c>
+      <c r="C16" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17">
         <v>160</v>
       </c>
-      <c r="B12" t="s">
-        <v>30</v>
-      </c>
-      <c r="C12" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3">
-      <c r="A13">
-        <v>160</v>
-      </c>
-      <c r="B13" t="s">
-        <v>31</v>
-      </c>
-      <c r="C13" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3">
-      <c r="A14">
+      <c r="B17">
+        <v>5.0390999999999998E-2</v>
+      </c>
+      <c r="C17" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18">
         <v>240</v>
       </c>
-      <c r="B14" t="s">
-        <v>32</v>
-      </c>
-      <c r="C14" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3">
-      <c r="A15">
-        <v>240</v>
-      </c>
-      <c r="B15" t="s">
-        <v>33</v>
-      </c>
-      <c r="C15" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3">
-      <c r="A16">
-        <v>240</v>
-      </c>
-      <c r="B16" t="s">
-        <v>34</v>
-      </c>
-      <c r="C16" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3">
-      <c r="A17">
-        <v>400</v>
-      </c>
-      <c r="B17" t="s">
-        <v>35</v>
-      </c>
-      <c r="C17" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3">
-      <c r="A18">
-        <v>400</v>
-      </c>
-      <c r="B18" t="s">
-        <v>36</v>
+      <c r="B18">
+        <v>8.7323899999999996E-2</v>
       </c>
       <c r="C18" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>400</v>
       </c>
-      <c r="B19" t="s">
-        <v>37</v>
+      <c r="B19">
+        <v>0.29321700000000001</v>
       </c>
       <c r="C19" t="s">
-        <v>21</v>
+        <v>6</v>
       </c>
     </row>
   </sheetData>
+  <sortState ref="A2:C19">
+    <sortCondition ref="A1"/>
+  </sortState>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <drawing r:id="rId1"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>

<commit_message>
[labb1] Tuffare diagram och förklaring av dessa.
</commit_message>
<xml_diff>
--- a/Execution.xlsx
+++ b/Execution.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="1620" yWindow="0" windowWidth="19440" windowHeight="12240" tabRatio="500"/>
+    <workbookView xWindow="1620" yWindow="0" windowWidth="7500" windowHeight="4920" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -351,21 +351,40 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="90840064"/>
-        <c:axId val="70574848"/>
+        <c:axId val="81313152"/>
+        <c:axId val="81319040"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="90840064"/>
+        <c:axId val="81313152"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="sv-SE"/>
+                  <a:t>Radie</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="70574848"/>
+        <c:crossAx val="81319040"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -373,18 +392,37 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="70574848"/>
+        <c:axId val="81319040"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
         <c:majorGridlines/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" vert="horz"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="sv-SE"/>
+                  <a:t>Exekveringstid</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="90840064"/>
+        <c:crossAx val="81313152"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -622,21 +660,40 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="32750592"/>
-        <c:axId val="32752384"/>
+        <c:axId val="81787520"/>
+        <c:axId val="88150400"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="32750592"/>
+        <c:axId val="81787520"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="sv-SE"/>
+                  <a:t>Kärnor</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="32752384"/>
+        <c:crossAx val="88150400"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -644,7 +701,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="32752384"/>
+        <c:axId val="88150400"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="0.30000000000000004"/>
@@ -652,11 +709,30 @@
         <c:delete val="0"/>
         <c:axPos val="l"/>
         <c:majorGridlines/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" vert="horz"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="sv-SE"/>
+                  <a:t>Exekveringstid</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="0"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="32750592"/>
+        <c:crossAx val="81787520"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1072,8 +1148,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+    <sheetView topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="K21" sqref="K21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1250,7 +1326,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C19"/>
   <sheetViews>
-    <sheetView topLeftCell="A8" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="K16" sqref="K16"/>
     </sheetView>
   </sheetViews>

</xml_diff>